<commit_message>
One number with +7
</commit_message>
<xml_diff>
--- a/numbers.xlsx
+++ b/numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Bot_for_TrueCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AA5D0C-E795-48D0-A526-9272E7B1C61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E35C1-DA52-488C-9C21-E0067D829B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1073" yWindow="1073" windowWidth="16875" windowHeight="10522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ФИО</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Гамаюнова Аделина</t>
   </si>
   <si>
-    <t>89842740104</t>
-  </si>
-  <si>
     <t>Ансимов Артём</t>
   </si>
   <si>
@@ -47,6 +44,12 @@
   </si>
   <si>
     <t>Кешикова Александра</t>
+  </si>
+  <si>
+    <t>89834626819</t>
+  </si>
+  <si>
+    <t>+79842740104</t>
   </si>
 </sst>
 </file>
@@ -416,12 +419,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.796875" customWidth="1"/>
     <col min="2" max="2" width="17.265625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -438,31 +441,31 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>89834626819</v>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>